<commit_message>
PBI model ready, all country data loaded, some indicators defined.
</commit_message>
<xml_diff>
--- a/country_file_name.xlsx
+++ b/country_file_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\WorldBank_databrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3253BFA4-FF01-45E2-9F2D-CFE69DAEA7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47062562-5709-4CE5-842C-0BF017567914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27855" yWindow="6690" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>country name</t>
   </si>
@@ -52,6 +52,102 @@
   </si>
   <si>
     <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>API_DZA_DS2_en_csv_v2_5753918.csv</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>API_AUS_DS2_en_csv_v2_5731277.csv</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>API_COG_DS2_en_csv_v2_5731397.csv</t>
+  </si>
+  <si>
+    <t>API_GHA_DS2_en_csv_v2_5702285.csv</t>
+  </si>
+  <si>
+    <t>API_IDN_DS2_en_csv_v2_5707985.csv</t>
+  </si>
+  <si>
+    <t>Congo, Rep.</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Venezuela, RB</t>
+  </si>
+  <si>
+    <t>API_KAZ_DS2_en_csv_v2_5731402.csv</t>
+  </si>
+  <si>
+    <t>API_LBY_DS2_en_csv_v2_5731400.csv</t>
+  </si>
+  <si>
+    <t>API_MEX_DS2_en_csv_v2_5795796.csv</t>
+  </si>
+  <si>
+    <t>API_NGA_DS2_en_csv_v2_5693925.csv</t>
+  </si>
+  <si>
+    <t>API_TUN_DS2_en_csv_v2_5731302.csv</t>
+  </si>
+  <si>
+    <t>API_TKM_DS2_en_csv_v2_5695641.csv</t>
+  </si>
+  <si>
+    <t>API_GBR_DS2_en_csv_v2_5731410.csv</t>
+  </si>
+  <si>
+    <t>API_USA_DS2_en_csv_v2_5730402.csv</t>
+  </si>
+  <si>
+    <t>API_VEN_DS2_en_csv_v2_5740096.csv</t>
+  </si>
+  <si>
+    <t>API_CIV_DS2_en_csv_v2_5758464.csv</t>
+  </si>
+  <si>
+    <t>API_PAK_DS2_en_csv_v2_5708202.csv</t>
   </si>
 </sst>
 </file>
@@ -108,8 +204,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}" name="country_file_name" displayName="country_file_name" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}" name="country_file_name" displayName="country_file_name" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{142A2605-CA5B-4670-84E3-5B79E25A6DA6}" name="country name"/>
     <tableColumn id="2" xr3:uid="{9DC20EFC-CD00-45EE-9065-798D74B0E5ED}" name="file name"/>
@@ -382,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
@@ -439,6 +535,182 @@
         <v>45156</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
This package now works as data browser. Last commit before branching for eni project.
</commit_message>
<xml_diff>
--- a/country_file_name.xlsx
+++ b/country_file_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\WorldBank_databrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47062562-5709-4CE5-842C-0BF017567914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF467C3-D0B9-4169-A0A4-AAF51AF8F041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>country name</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>API_PAK_DS2_en_csv_v2_5708202.csv</t>
+  </si>
+  <si>
+    <t>data type</t>
+  </si>
+  <si>
+    <t>World Bank</t>
   </si>
 </sst>
 </file>
@@ -204,10 +210,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}" name="country_file_name" displayName="country_file_name" ref="A1:C20" totalsRowShown="0">
-  <autoFilter ref="A1:C20" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}" name="country_file_name" displayName="country_file_name" ref="A1:D20" totalsRowShown="0">
+  <autoFilter ref="A1:D20" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{142A2605-CA5B-4670-84E3-5B79E25A6DA6}" name="country name"/>
+    <tableColumn id="4" xr3:uid="{C33E7F6C-9B1B-45EF-812C-AFA5F992BE37}" name="data type"/>
     <tableColumn id="2" xr3:uid="{9DC20EFC-CD00-45EE-9065-798D74B0E5ED}" name="file name"/>
     <tableColumn id="3" xr3:uid="{85FE2A77-EEAD-430B-BB3E-EA1B471515E1}" name="download date"/>
   </tableColumns>
@@ -478,236 +485,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="36.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>45154</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>45154</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>45156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iea data files link organized and first IT and EG data added. Data file names list reorganized and updated in the model. Indicators selection file updated.
</commit_message>
<xml_diff>
--- a/country_file_name.xlsx
+++ b/country_file_name.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\WorldBank_databrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF467C3-D0B9-4169-A0A4-AAF51AF8F041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17E996A-C8C9-47D7-ABFD-F87923ED8C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="2400" windowWidth="24795" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="country_file_name" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>country name</t>
   </si>
   <si>
-    <t>file name</t>
-  </si>
-  <si>
     <t>Italy</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>Egypt, Arab Rep.</t>
   </si>
   <si>
-    <t>download date</t>
-  </si>
-  <si>
     <t>API_MOZ_DS2_en_csv_v2_5742130.csv</t>
   </si>
   <si>
@@ -150,10 +144,16 @@
     <t>API_PAK_DS2_en_csv_v2_5708202.csv</t>
   </si>
   <si>
-    <t>data type</t>
-  </si>
-  <si>
-    <t>World Bank</t>
+    <t>country data wb</t>
+  </si>
+  <si>
+    <t>country data iea</t>
+  </si>
+  <si>
+    <t>EG_iea.xlsx</t>
+  </si>
+  <si>
+    <t>IT_iea.xlsx</t>
   </si>
 </sst>
 </file>
@@ -189,9 +189,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,13 +209,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}" name="country_file_name" displayName="country_file_name" ref="A1:D20" totalsRowShown="0">
-  <autoFilter ref="A1:D20" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}" name="country_file_name" displayName="country_file_name" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{0E410B69-C5EB-493B-AA86-08C48456F9C3}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{142A2605-CA5B-4670-84E3-5B79E25A6DA6}" name="country name"/>
-    <tableColumn id="4" xr3:uid="{C33E7F6C-9B1B-45EF-812C-AFA5F992BE37}" name="data type"/>
-    <tableColumn id="2" xr3:uid="{9DC20EFC-CD00-45EE-9065-798D74B0E5ED}" name="file name"/>
-    <tableColumn id="3" xr3:uid="{85FE2A77-EEAD-430B-BB3E-EA1B471515E1}" name="download date"/>
+    <tableColumn id="2" xr3:uid="{9DC20EFC-CD00-45EE-9065-798D74B0E5ED}" name="country data wb"/>
+    <tableColumn id="4" xr3:uid="{C33E7F6C-9B1B-45EF-812C-AFA5F992BE37}" name="country data iea"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -485,297 +483,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="36.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B20" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="1">
-        <v>45156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
table naming adjusted. dummy eni_project list and data files added for starting structuring the algorithm. energy data for Australia added.
</commit_message>
<xml_diff>
--- a/country_file_name.xlsx
+++ b/country_file_name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\WorldBank_databrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17E996A-C8C9-47D7-ABFD-F87923ED8C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEF2021-E370-44D6-A717-E4B846FC79D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="2400" windowWidth="24795" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34600" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country_file_name" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>country name</t>
   </si>
@@ -150,10 +150,13 @@
     <t>country data iea</t>
   </si>
   <si>
-    <t>EG_iea.xlsx</t>
-  </si>
-  <si>
-    <t>IT_iea.xlsx</t>
+    <t>IT.csv</t>
+  </si>
+  <si>
+    <t>EG.csv</t>
+  </si>
+  <si>
+    <t>AU.csv</t>
   </si>
 </sst>
 </file>
@@ -486,17 +489,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -515,10 +518,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -526,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -537,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -545,15 +548,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -561,7 +567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -569,7 +575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -577,7 +583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -585,7 +591,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -593,7 +599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -601,7 +607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -609,7 +615,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -617,7 +623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -625,7 +631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -633,7 +639,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -641,7 +647,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -649,7 +655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -657,7 +663,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Metadata embedded into readme. Enegy data for all countries included.
</commit_message>
<xml_diff>
--- a/country_file_name.xlsx
+++ b/country_file_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\WorldBank_databrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEF2021-E370-44D6-A717-E4B846FC79D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395BA1ED-5D50-4CB0-9789-F0477AB761E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34600" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country_file_name" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>country name</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>AU.csv</t>
+  </si>
+  <si>
+    <t>ID.csv</t>
+  </si>
+  <si>
+    <t>KZ.csv</t>
+  </si>
+  <si>
+    <t>TM.csv</t>
   </si>
 </sst>
 </file>
@@ -489,17 +498,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" customWidth="1"/>
-    <col min="2" max="2" width="43.81640625" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +519,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -521,7 +530,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -532,7 +541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -540,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -548,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -559,7 +568,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -567,7 +576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -575,23 +584,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -599,7 +614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -607,7 +622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -615,7 +630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -623,15 +638,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -639,7 +657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -647,7 +665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -655,7 +673,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -663,7 +681,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Energy data revised and corrected.
</commit_message>
<xml_diff>
--- a/country_file_name.xlsx
+++ b/country_file_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\WorldBank_databrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395BA1ED-5D50-4CB0-9789-F0477AB761E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6464DD-4DCB-40FD-A870-09D159565BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17430" yWindow="2600" windowWidth="14750" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country_file_name" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>country name</t>
   </si>
@@ -166,6 +166,45 @@
   </si>
   <si>
     <t>TM.csv</t>
+  </si>
+  <si>
+    <t>MZ.csv</t>
+  </si>
+  <si>
+    <t>LY.csv</t>
+  </si>
+  <si>
+    <t>MX.csv</t>
+  </si>
+  <si>
+    <t>TN.csv</t>
+  </si>
+  <si>
+    <t>PK.csv</t>
+  </si>
+  <si>
+    <t>DZ.csv</t>
+  </si>
+  <si>
+    <t>CG.csv</t>
+  </si>
+  <si>
+    <t>GH.csv</t>
+  </si>
+  <si>
+    <t>NG.csv</t>
+  </si>
+  <si>
+    <t>GB.csv</t>
+  </si>
+  <si>
+    <t>US.csv</t>
+  </si>
+  <si>
+    <t>VE.csv</t>
+  </si>
+  <si>
+    <t>CI.csv</t>
   </si>
 </sst>
 </file>
@@ -498,17 +537,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -530,7 +569,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -541,23 +580,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -568,23 +613,29 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -595,7 +646,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -606,39 +657,51 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -649,44 +712,59 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>